<commit_message>
Revert "Revert "Starting point""
This reverts commit ec1377b4dcc64a6c0f51041d34e8f70536ea4925.
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-OperationOutcome.xlsx
+++ b/output/carin-rtpbc-OperationOutcome.xlsx
@@ -150,7 +150,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Grouping is handled through multiple repetitions from whatever context references the outcomes (no specific grouper required)</t>
@@ -165,7 +165,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -197,6 +197,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
     <t>OperationOutcome.implicitRules</t>
   </si>
   <si>
@@ -319,6 +323,10 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
     <t>OperationOutcome.modifierExtension</t>
   </si>
   <si>
@@ -348,10 +356,6 @@
     <t>An error, warning, or information message that results from a system action.</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
-  </si>
-  <si>
     <t>AcknowledgementDetail or Observation[classCode="ALRT" and moodCode="EVN"]</t>
   </si>
   <si>
@@ -359,10 +363,6 @@
   </si>
   <si>
     <t>OperationOutcome.issue.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
   </si>
   <si>
     <t>Unique id for inter-element referencing</t>
@@ -424,7 +424,7 @@
     <t>How the issue affects the success of the action.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/issue-severity|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/issue-severity|4.0.1</t>
   </si>
   <si>
     <t>./typeCode[parent::AcknowledgmentDetail] or unique(./inboundRelationship[parent::Observation and typeCode='SUBJ' and isNormalActRelationship()]/source[classCode="OBS" and moodCode="EVN" and implies(code, ActCode#SEV and isNormalAct())/value[xsi:type="CD"]</t>
@@ -449,7 +449,7 @@
     <t>A code that describes the type of issue.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/issue-type|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/issue-type|4.0.1</t>
   </si>
   <si>
     <t>./code</t>
@@ -1149,7 +1149,7 @@
         <v>38</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>38</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1183,16 +1183,16 @@
         <v>48</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1242,7 +1242,7 @@
         <v>38</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>39</v>
@@ -1254,7 +1254,7 @@
         <v>38</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>38</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1288,16 +1288,16 @@
         <v>38</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1323,13 +1323,13 @@
         <v>38</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>38</v>
@@ -1347,7 +1347,7 @@
         <v>38</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>39</v>
@@ -1359,7 +1359,7 @@
         <v>38</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>38</v>
@@ -1370,11 +1370,11 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1393,16 +1393,16 @@
         <v>38</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1452,7 +1452,7 @@
         <v>38</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>39</v>
@@ -1464,10 +1464,10 @@
         <v>38</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>38</v>
@@ -1475,11 +1475,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1498,16 +1498,16 @@
         <v>38</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1557,7 +1557,7 @@
         <v>38</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>39</v>
@@ -1572,7 +1572,7 @@
         <v>38</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>38</v>
@@ -1580,11 +1580,11 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -1603,16 +1603,16 @@
         <v>38</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -1662,7 +1662,7 @@
         <v>38</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>39</v>
@@ -1674,10 +1674,10 @@
         <v>38</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>38</v>
@@ -1685,11 +1685,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -1708,19 +1708,19 @@
         <v>38</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>38</v>
@@ -1769,7 +1769,7 @@
         <v>38</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -1781,10 +1781,10 @@
         <v>38</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>38</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1815,13 +1815,13 @@
         <v>48</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1872,7 +1872,7 @@
         <v>38</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>47</v>
@@ -1884,18 +1884,18 @@
         <v>38</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1918,7 +1918,7 @@
         <v>38</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>111</v>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2021,16 +2021,16 @@
         <v>38</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s" s="2">
         <v>116</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2092,7 +2092,7 @@
         <v>38</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>114</v>
@@ -2126,7 +2126,7 @@
         <v>48</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K14" t="s" s="2">
         <v>120</v>
@@ -2135,10 +2135,10 @@
         <v>121</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>38</v>
@@ -2199,10 +2199,10 @@
         <v>38</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>38</v>
@@ -2233,7 +2233,7 @@
         <v>48</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K15" t="s" s="2">
         <v>124</v>
@@ -2306,7 +2306,7 @@
         <v>38</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>131</v>
@@ -2340,7 +2340,7 @@
         <v>48</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>134</v>
@@ -2411,7 +2411,7 @@
         <v>38</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>139</v>
@@ -2516,7 +2516,7 @@
         <v>38</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>139</v>
@@ -2550,7 +2550,7 @@
         <v>48</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="K18" t="s" s="2">
         <v>151</v>
@@ -2621,7 +2621,7 @@
         <v>38</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>154</v>
@@ -2655,7 +2655,7 @@
         <v>48</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>157</v>
@@ -2728,7 +2728,7 @@
         <v>38</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>161</v>
@@ -2762,7 +2762,7 @@
         <v>48</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>164</v>
@@ -2835,7 +2835,7 @@
         <v>38</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>161</v>

</xml_diff>